<commit_message>
Generate multiple docx file
</commit_message>
<xml_diff>
--- a/HeroAcheiver.xlsx
+++ b/HeroAcheiver.xlsx
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="46">
   <si>
     <t>S No</t>
   </si>
@@ -206,10 +206,13 @@
     <t>Hero Acheiver</t>
   </si>
   <si>
-    <t>dfsfjkaj</t>
+    <t>Purchased Date</t>
   </si>
   <si>
-    <t>Purchased Date</t>
+    <t>testing1</t>
+  </si>
+  <si>
+    <t>testing2</t>
   </si>
 </sst>
 </file>
@@ -821,10 +824,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -865,7 +868,7 @@
         <v>39</v>
       </c>
       <c r="I1" s="30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="35" customFormat="1">
@@ -901,9 +904,9 @@
         <v>43495</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="35" customFormat="1">
+    <row r="3" spans="1:9">
       <c r="A3" s="31" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B3" s="32">
         <v>69959</v>
@@ -931,6 +934,39 @@
         <v>40</v>
       </c>
       <c r="I3" s="17">
+        <v>43495</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="32">
+        <v>69959</v>
+      </c>
+      <c r="C4" s="32">
+        <v>1140</v>
+      </c>
+      <c r="D4" s="33">
+        <f>SUM(B4,C4)</f>
+        <v>71099</v>
+      </c>
+      <c r="E4" s="33">
+        <f>Services!I3</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="32">
+        <f>Fuel!I3</f>
+        <v>0</v>
+      </c>
+      <c r="G4" s="33">
+        <f>D4+E4+F4</f>
+        <v>71099</v>
+      </c>
+      <c r="H4" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="I4" s="17">
         <v>43495</v>
       </c>
     </row>
@@ -8551,7 +8587,7 @@
       </c>
       <c r="H2" s="6">
         <f ca="1">DATEDIF(TODAY(),Services!F6,"D")</f>
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1">
@@ -8625,7 +8661,7 @@
       </c>
       <c r="H6" s="13">
         <f ca="1">H4/H2</f>
-        <v>52.912820512820524</v>
+        <v>54.30526315789475</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1">

</xml_diff>